<commit_message>
chore: agregar EV_WBS actualizada
</commit_message>
<xml_diff>
--- a/Plantilla_EV_WBS.xlsx
+++ b/Plantilla_EV_WBS.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="87">
   <si>
     <t>Plantilla EV + WBS (versión simple)</t>
   </si>
@@ -124,85 +124,121 @@
     <t>Alex García Castañeda</t>
   </si>
   <si>
+    <t>FINALIZADA</t>
+  </si>
+  <si>
+    <t>1.4.3</t>
+  </si>
+  <si>
+    <t>14- Diseñar estructura de memoria contextual</t>
+  </si>
+  <si>
+    <t>1.1.2</t>
+  </si>
+  <si>
+    <t>16 - Endpoint para registro de conversaciones con emociones</t>
+  </si>
+  <si>
+    <t>17 - Consultar historial conversacional por usuario y fecha</t>
+  </si>
+  <si>
+    <t>Juan Manuel Arango Rodas</t>
+  </si>
+  <si>
+    <t>15 - Crear endpoints REST para gestión de usuarios</t>
+  </si>
+  <si>
+    <t>Tina María Torres Tascón</t>
+  </si>
+  <si>
+    <t>1.1.1</t>
+  </si>
+  <si>
+    <t>26 - Implementación de capa de acceso a datos (DAO / Repository)</t>
+  </si>
+  <si>
+    <t>29 -  Generación y gestión de embeddings</t>
+  </si>
+  <si>
+    <t>1.1.3</t>
+  </si>
+  <si>
+    <t>27 - Configuración del entorno local con Docker</t>
+  </si>
+  <si>
+    <t>24- Definición de arquitectura lógica y técnica</t>
+  </si>
+  <si>
+    <t>Stiven Henao Aricapa</t>
+  </si>
+  <si>
+    <t>25- Diseño del modelo de datos relacional y vectorial</t>
+  </si>
+  <si>
+    <t>Víctor Manuel Hernández Ortíz</t>
+  </si>
+  <si>
+    <t>1.3.1</t>
+  </si>
+  <si>
+    <t>28- Configurar conexión con el modelo Gemini</t>
+  </si>
+  <si>
+    <t>1.4.1, 1.3.2</t>
+  </si>
+  <si>
+    <t>12- Diseño del pipeline de conversación</t>
+  </si>
+  <si>
+    <t>Juan Sebastían Gómez Agudelo</t>
+  </si>
+  <si>
+    <t>11- Implementar RAG básico con artículos psicológicos</t>
+  </si>
+  <si>
+    <t>Memoria contextual integrada al flujo conversacional + RAG</t>
+  </si>
+  <si>
+    <t>Frontend de gestión de usuarios</t>
+  </si>
+  <si>
+    <t>Sebastián Gómez Agudelo</t>
+  </si>
+  <si>
+    <t>Exportación de reportes PDF del historial conversacional</t>
+  </si>
+  <si>
+    <t>Pruebas iniciales de conexión con hardware</t>
+  </si>
+  <si>
+    <t>Mejorar fluidez y velocidad de conversación</t>
+  </si>
+  <si>
+    <t>Manuel Gómez</t>
+  </si>
+  <si>
+    <t>EN CURSO</t>
+  </si>
+  <si>
+    <t>1.6.2</t>
+  </si>
+  <si>
+    <t>Seguridad básica: cifrado y protección de datos</t>
+  </si>
+  <si>
+    <t>1.2.3</t>
+  </si>
+  <si>
+    <t>Integración final con hardware (Micrófono y Voz)</t>
+  </si>
+  <si>
     <t>POR HACER</t>
   </si>
   <si>
-    <t>1.4.3</t>
-  </si>
-  <si>
-    <t>14- Diseñar estructura de memoria contextual</t>
-  </si>
-  <si>
-    <t>1.1.2</t>
-  </si>
-  <si>
-    <t>16 - Endpoint para registro de conversaciones con emociones</t>
-  </si>
-  <si>
-    <t>17 - Consultar historial conversacional por usuario y fecha</t>
-  </si>
-  <si>
-    <t>Juan Manuel Arango Rodas</t>
-  </si>
-  <si>
-    <t>EN CURSO</t>
-  </si>
-  <si>
-    <t>15 - Crear endpoints REST para gestión de usuarios</t>
-  </si>
-  <si>
-    <t>Tina María Torres Tascón</t>
-  </si>
-  <si>
-    <t>1.1.1</t>
-  </si>
-  <si>
-    <t>26 - Implementación de capa de acceso a datos (DAO / Repository)</t>
-  </si>
-  <si>
-    <t>29 -  Generación y gestión de embeddings</t>
-  </si>
-  <si>
-    <t>1.1.3</t>
-  </si>
-  <si>
-    <t>27 - Configuración del entorno local con Docker</t>
-  </si>
-  <si>
-    <t>24- Definición de arquitectura lógica y técnica</t>
-  </si>
-  <si>
-    <t>Stiven Henao Aricapa</t>
-  </si>
-  <si>
-    <t>FINALIZADA</t>
-  </si>
-  <si>
-    <t>25- Diseño del modelo de datos relacional y vectorial</t>
-  </si>
-  <si>
-    <t>Víctor Manuel Hernández Ortíz</t>
-  </si>
-  <si>
-    <t>1.3.1</t>
-  </si>
-  <si>
-    <t>28- Configurar conexión con el modelo Gemini</t>
-  </si>
-  <si>
-    <t>1.4.1, 1.3.2</t>
-  </si>
-  <si>
-    <t>12- Diseño del pipeline de conversación</t>
-  </si>
-  <si>
-    <t>Juan Sebastían Gómez Agudelo</t>
-  </si>
-  <si>
-    <t>EN REVISIÓN</t>
-  </si>
-  <si>
-    <t>11- Implementar RAG básico con artículos psicológicos</t>
+    <t>1.5.2</t>
+  </si>
+  <si>
+    <t>Pruebas finales + documentación entregable</t>
   </si>
   <si>
     <t>Métrica</t>
@@ -245,10 +281,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
     <numFmt numFmtId="165" formatCode="d-m-yyyy"/>
     <numFmt numFmtId="166" formatCode="dd-mm-yyyy"/>
+    <numFmt numFmtId="167" formatCode="d.m"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -293,7 +330,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -314,32 +351,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB7B7B7"/>
-        <bgColor rgb="FFB7B7B7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF6FA8DC"/>
-        <bgColor rgb="FF6FA8DC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF93C47D"/>
         <bgColor rgb="FF93C47D"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor theme="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC27BA0"/>
-        <bgColor rgb="FFC27BA0"/>
       </patternFill>
     </fill>
   </fills>
@@ -407,17 +420,17 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
@@ -455,9 +468,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
+      <xdr:colOff>657225</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="19507200" cy="2076450"/>
     <xdr:pic>
@@ -786,7 +799,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="7">
-        <v>1000.0</v>
+        <v>100000.0</v>
       </c>
     </row>
     <row r="3">
@@ -891,34 +904,36 @@
       </c>
       <c r="E2" s="14">
         <f>Config!$B$2</f>
-        <v>1000</v>
+        <v>100000</v>
       </c>
       <c r="F2" s="14">
-        <f t="shared" ref="F2:F21" si="1">D2*E2</f>
-        <v>3000</v>
+        <f t="shared" ref="F2:F14" si="1">D2*E2</f>
+        <v>300000</v>
       </c>
       <c r="G2" s="15">
         <v>1.0</v>
       </c>
       <c r="H2" s="14">
-        <f t="shared" ref="H2:H21" si="2">F2*G2</f>
-        <v>3000</v>
+        <f t="shared" ref="H2:H14" si="2">F2*G2</f>
+        <v>300000</v>
       </c>
       <c r="I2" s="15">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J2" s="14">
-        <f t="shared" ref="J2:J21" si="3">F2*I2</f>
+        <f t="shared" ref="J2:J14" si="3">F2*I2</f>
+        <v>300000</v>
+      </c>
+      <c r="K2" s="15">
+        <v>350000.0</v>
+      </c>
+      <c r="L2" s="14">
+        <f t="shared" ref="L2:L14" si="4">J2-H2</f>
         <v>0</v>
       </c>
-      <c r="K2" s="12"/>
-      <c r="L2" s="14">
-        <f t="shared" ref="L2:L21" si="4">J2-H2</f>
-        <v>-3000</v>
-      </c>
       <c r="M2" s="14">
-        <f t="shared" ref="M2:M21" si="5">J2-K2</f>
-        <v>0</v>
+        <f t="shared" ref="M2:M14" si="5">J2-K2</f>
+        <v>-50000</v>
       </c>
       <c r="N2" s="15" t="s">
         <v>35</v>
@@ -930,9 +945,11 @@
         <v>45951.0</v>
       </c>
       <c r="Q2" s="18">
-        <v>45965.0</v>
-      </c>
-      <c r="R2" s="12"/>
+        <v>45972.0</v>
+      </c>
+      <c r="R2" s="17">
+        <v>45957.0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="10" t="s">
@@ -947,34 +964,36 @@
       </c>
       <c r="E3" s="14">
         <f>Config!$B$2</f>
-        <v>1000</v>
+        <v>100000</v>
       </c>
       <c r="F3" s="14">
         <f t="shared" si="1"/>
-        <v>8000</v>
+        <v>800000</v>
       </c>
       <c r="G3" s="15">
         <v>1.0</v>
       </c>
       <c r="H3" s="14">
         <f t="shared" si="2"/>
-        <v>8000</v>
+        <v>800000</v>
       </c>
       <c r="I3" s="15">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J3" s="14">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K3" s="12"/>
+        <v>800000</v>
+      </c>
+      <c r="K3" s="15">
+        <v>300000.0</v>
+      </c>
       <c r="L3" s="14">
         <f t="shared" si="4"/>
-        <v>-8000</v>
+        <v>0</v>
       </c>
       <c r="M3" s="14">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>500000</v>
       </c>
       <c r="N3" s="15" t="s">
         <v>35</v>
@@ -986,9 +1005,11 @@
         <v>45951.0</v>
       </c>
       <c r="Q3" s="18">
-        <v>45965.0</v>
-      </c>
-      <c r="R3" s="12"/>
+        <v>45973.0</v>
+      </c>
+      <c r="R3" s="17">
+        <v>45958.0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="10" t="s">
@@ -1003,34 +1024,36 @@
       </c>
       <c r="E4" s="14">
         <f>Config!$B$2</f>
-        <v>1000</v>
+        <v>100000</v>
       </c>
       <c r="F4" s="14">
         <f t="shared" si="1"/>
-        <v>5000</v>
+        <v>500000</v>
       </c>
       <c r="G4" s="15">
         <v>1.0</v>
       </c>
       <c r="H4" s="14">
         <f t="shared" si="2"/>
-        <v>5000</v>
+        <v>500000</v>
       </c>
       <c r="I4" s="15">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J4" s="14">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K4" s="12"/>
+        <v>500000</v>
+      </c>
+      <c r="K4" s="15">
+        <v>200000.0</v>
+      </c>
       <c r="L4" s="14">
         <f t="shared" si="4"/>
-        <v>-5000</v>
+        <v>0</v>
       </c>
       <c r="M4" s="14">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>300000</v>
       </c>
       <c r="N4" s="15" t="s">
         <v>35</v>
@@ -1042,9 +1065,11 @@
         <v>45951.0</v>
       </c>
       <c r="Q4" s="18">
-        <v>45965.0</v>
-      </c>
-      <c r="R4" s="12"/>
+        <v>45974.0</v>
+      </c>
+      <c r="R4" s="17">
+        <v>45959.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="10" t="s">
@@ -1059,55 +1084,59 @@
       </c>
       <c r="E5" s="14">
         <f>Config!$B$2</f>
-        <v>1000</v>
+        <v>100000</v>
       </c>
       <c r="F5" s="14">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>300000</v>
       </c>
       <c r="G5" s="15">
         <v>1.0</v>
       </c>
       <c r="H5" s="14">
         <f t="shared" si="2"/>
-        <v>3000</v>
+        <v>300000</v>
       </c>
       <c r="I5" s="15">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J5" s="14">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K5" s="12"/>
+        <v>300000</v>
+      </c>
+      <c r="K5" s="15">
+        <v>240000.0</v>
+      </c>
       <c r="L5" s="14">
         <f t="shared" si="4"/>
-        <v>-3000</v>
+        <v>0</v>
       </c>
       <c r="M5" s="14">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>60000</v>
       </c>
       <c r="N5" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="O5" s="19" t="s">
-        <v>43</v>
+      <c r="O5" s="16" t="s">
+        <v>36</v>
       </c>
       <c r="P5" s="17">
         <v>45951.0</v>
       </c>
       <c r="Q5" s="18">
-        <v>45965.0</v>
-      </c>
-      <c r="R5" s="12"/>
+        <v>45975.0</v>
+      </c>
+      <c r="R5" s="17">
+        <v>45959.0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="10" t="s">
         <v>39</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" s="12"/>
       <c r="D6" s="13">
@@ -1115,55 +1144,59 @@
       </c>
       <c r="E6" s="14">
         <f>Config!$B$2</f>
-        <v>1000</v>
+        <v>100000</v>
       </c>
       <c r="F6" s="14">
         <f t="shared" si="1"/>
-        <v>5000</v>
+        <v>500000</v>
       </c>
       <c r="G6" s="15">
         <v>1.0</v>
       </c>
       <c r="H6" s="14">
         <f t="shared" si="2"/>
-        <v>5000</v>
+        <v>500000</v>
       </c>
       <c r="I6" s="15">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J6" s="14">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K6" s="12"/>
+        <v>500000</v>
+      </c>
+      <c r="K6" s="15">
+        <v>200000.0</v>
+      </c>
       <c r="L6" s="14">
         <f t="shared" si="4"/>
-        <v>-5000</v>
+        <v>0</v>
       </c>
       <c r="M6" s="14">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>300000</v>
       </c>
       <c r="N6" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="O6" s="19" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="O6" s="16" t="s">
+        <v>36</v>
       </c>
       <c r="P6" s="17">
         <v>45951.0</v>
       </c>
       <c r="Q6" s="18">
-        <v>45965.0</v>
-      </c>
-      <c r="R6" s="12"/>
+        <v>45976.0</v>
+      </c>
+      <c r="R6" s="17">
+        <v>45959.0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>46</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>47</v>
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="13">
@@ -1171,55 +1204,59 @@
       </c>
       <c r="E7" s="14">
         <f>Config!$B$2</f>
-        <v>1000</v>
+        <v>100000</v>
       </c>
       <c r="F7" s="14">
         <f t="shared" si="1"/>
-        <v>5000</v>
+        <v>500000</v>
       </c>
       <c r="G7" s="15">
         <v>1.0</v>
       </c>
       <c r="H7" s="14">
         <f t="shared" si="2"/>
-        <v>5000</v>
+        <v>500000</v>
       </c>
       <c r="I7" s="15">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J7" s="14">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K7" s="12"/>
+        <v>500000</v>
+      </c>
+      <c r="K7" s="15">
+        <v>250000.0</v>
+      </c>
       <c r="L7" s="14">
         <f t="shared" si="4"/>
-        <v>-5000</v>
+        <v>0</v>
       </c>
       <c r="M7" s="14">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>250000</v>
       </c>
       <c r="N7" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="19" t="s">
-        <v>43</v>
+      <c r="O7" s="16" t="s">
+        <v>36</v>
       </c>
       <c r="P7" s="17">
         <v>45951.0</v>
       </c>
       <c r="Q7" s="18">
-        <v>45965.0</v>
-      </c>
-      <c r="R7" s="12"/>
+        <v>45977.0</v>
+      </c>
+      <c r="R7" s="18">
+        <v>45962.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="10" t="s">
         <v>37</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="13">
@@ -1227,55 +1264,59 @@
       </c>
       <c r="E8" s="14">
         <f>Config!$B$2</f>
-        <v>1000</v>
+        <v>100000</v>
       </c>
       <c r="F8" s="14">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>200000</v>
       </c>
       <c r="G8" s="15">
         <v>1.0</v>
       </c>
       <c r="H8" s="14">
         <f t="shared" si="2"/>
-        <v>2000</v>
+        <v>200000</v>
       </c>
       <c r="I8" s="15">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J8" s="14">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K8" s="12"/>
+        <v>200000</v>
+      </c>
+      <c r="K8" s="15">
+        <v>400000.0</v>
+      </c>
       <c r="L8" s="14">
         <f t="shared" si="4"/>
-        <v>-2000</v>
+        <v>0</v>
       </c>
       <c r="M8" s="14">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-200000</v>
       </c>
       <c r="N8" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="O8" s="19" t="s">
-        <v>43</v>
+      <c r="O8" s="16" t="s">
+        <v>36</v>
       </c>
       <c r="P8" s="17">
         <v>45951.0</v>
       </c>
       <c r="Q8" s="18">
-        <v>45965.0</v>
-      </c>
-      <c r="R8" s="12"/>
+        <v>45978.0</v>
+      </c>
+      <c r="R8" s="18">
+        <v>45962.0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>49</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>50</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="13">
@@ -1283,30 +1324,32 @@
       </c>
       <c r="E9" s="14">
         <f>Config!$B$2</f>
-        <v>1000</v>
+        <v>100000</v>
       </c>
       <c r="F9" s="14">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>200000</v>
       </c>
       <c r="G9" s="15">
         <v>1.0</v>
       </c>
       <c r="H9" s="14">
         <f t="shared" si="2"/>
-        <v>2000</v>
+        <v>200000</v>
       </c>
       <c r="I9" s="15">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J9" s="14">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K9" s="12"/>
+        <v>200000</v>
+      </c>
+      <c r="K9" s="15">
+        <v>200000.0</v>
+      </c>
       <c r="L9" s="14">
         <f t="shared" si="4"/>
-        <v>-2000</v>
+        <v>0</v>
       </c>
       <c r="M9" s="14">
         <f t="shared" si="5"/>
@@ -1315,23 +1358,25 @@
       <c r="N9" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="O9" s="19" t="s">
-        <v>43</v>
+      <c r="O9" s="16" t="s">
+        <v>36</v>
       </c>
       <c r="P9" s="17">
         <v>45951.0</v>
       </c>
       <c r="Q9" s="18">
-        <v>45965.0</v>
-      </c>
-      <c r="R9" s="12"/>
+        <v>45979.0</v>
+      </c>
+      <c r="R9" s="18">
+        <v>45962.0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="10" t="s">
         <v>39</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="13">
@@ -1339,46 +1384,48 @@
       </c>
       <c r="E10" s="14">
         <f>Config!$B$2</f>
-        <v>1000</v>
+        <v>100000</v>
       </c>
       <c r="F10" s="14">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>300000</v>
       </c>
       <c r="G10" s="15">
         <v>1.0</v>
       </c>
       <c r="H10" s="14">
         <f t="shared" si="2"/>
-        <v>3000</v>
+        <v>300000</v>
       </c>
       <c r="I10" s="15">
         <v>1.0</v>
       </c>
       <c r="J10" s="14">
         <f t="shared" si="3"/>
-        <v>3000</v>
-      </c>
-      <c r="K10" s="12"/>
+        <v>300000</v>
+      </c>
+      <c r="K10" s="15">
+        <v>240000.0</v>
+      </c>
       <c r="L10" s="14">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M10" s="14">
         <f t="shared" si="5"/>
-        <v>3000</v>
+        <v>60000</v>
       </c>
       <c r="N10" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="O10" s="20" t="s">
-        <v>53</v>
+        <v>51</v>
+      </c>
+      <c r="O10" s="16" t="s">
+        <v>36</v>
       </c>
       <c r="P10" s="17">
         <v>45951.0</v>
       </c>
       <c r="Q10" s="18">
-        <v>45965.0</v>
+        <v>45980.0</v>
       </c>
       <c r="R10" s="17">
         <v>45956.0</v>
@@ -1386,10 +1433,10 @@
     </row>
     <row r="11">
       <c r="A11" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C11" s="12"/>
       <c r="D11" s="13">
@@ -1397,46 +1444,48 @@
       </c>
       <c r="E11" s="14">
         <f>Config!$B$2</f>
-        <v>1000</v>
+        <v>100000</v>
       </c>
       <c r="F11" s="14">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>300000</v>
       </c>
       <c r="G11" s="15">
         <v>1.0</v>
       </c>
       <c r="H11" s="14">
         <f t="shared" si="2"/>
-        <v>3000</v>
+        <v>300000</v>
       </c>
       <c r="I11" s="15">
         <v>1.0</v>
       </c>
       <c r="J11" s="14">
         <f t="shared" si="3"/>
-        <v>3000</v>
-      </c>
-      <c r="K11" s="12"/>
+        <v>300000</v>
+      </c>
+      <c r="K11" s="15">
+        <v>290000.0</v>
+      </c>
       <c r="L11" s="14">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M11" s="14">
         <f t="shared" si="5"/>
-        <v>3000</v>
+        <v>10000</v>
       </c>
       <c r="N11" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="O11" s="20" t="s">
         <v>53</v>
+      </c>
+      <c r="O11" s="16" t="s">
+        <v>36</v>
       </c>
       <c r="P11" s="17">
         <v>45951.0</v>
       </c>
       <c r="Q11" s="18">
-        <v>45965.0</v>
+        <v>45981.0</v>
       </c>
       <c r="R11" s="17">
         <v>45956.0</v>
@@ -1444,10 +1493,10 @@
     </row>
     <row r="12">
       <c r="A12" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="13">
@@ -1455,55 +1504,59 @@
       </c>
       <c r="E12" s="14">
         <f>Config!$B$2</f>
-        <v>1000</v>
+        <v>100000</v>
       </c>
       <c r="F12" s="14">
         <f t="shared" si="1"/>
-        <v>5000</v>
+        <v>500000</v>
       </c>
       <c r="G12" s="15">
         <v>1.0</v>
       </c>
       <c r="H12" s="14">
         <f t="shared" si="2"/>
-        <v>5000</v>
+        <v>500000</v>
       </c>
       <c r="I12" s="15">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J12" s="14">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K12" s="12"/>
+        <v>500000</v>
+      </c>
+      <c r="K12" s="15">
+        <v>190000.0</v>
+      </c>
       <c r="L12" s="14">
         <f t="shared" si="4"/>
-        <v>-5000</v>
+        <v>0</v>
       </c>
       <c r="M12" s="14">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>310000</v>
       </c>
       <c r="N12" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="O12" s="21" t="s">
-        <v>43</v>
+        <v>51</v>
+      </c>
+      <c r="O12" s="16" t="s">
+        <v>36</v>
       </c>
       <c r="P12" s="17">
         <v>45951.0</v>
       </c>
       <c r="Q12" s="18">
-        <v>45965.0</v>
-      </c>
-      <c r="R12" s="12"/>
+        <v>45982.0</v>
+      </c>
+      <c r="R12" s="18">
+        <v>45966.0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C13" s="12"/>
       <c r="D13" s="13">
@@ -1511,55 +1564,59 @@
       </c>
       <c r="E13" s="14">
         <f>Config!$B$2</f>
-        <v>1000</v>
+        <v>100000</v>
       </c>
       <c r="F13" s="14">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>200000</v>
       </c>
       <c r="G13" s="15">
         <v>1.0</v>
       </c>
       <c r="H13" s="14">
         <f t="shared" si="2"/>
-        <v>2000</v>
+        <v>200000</v>
       </c>
       <c r="I13" s="15">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J13" s="14">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K13" s="12"/>
+        <v>200000</v>
+      </c>
+      <c r="K13" s="15">
+        <v>300000.0</v>
+      </c>
       <c r="L13" s="14">
         <f t="shared" si="4"/>
-        <v>-2000</v>
+        <v>0</v>
       </c>
       <c r="M13" s="14">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-100000</v>
       </c>
       <c r="N13" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="O13" s="22" t="s">
-        <v>61</v>
+        <v>58</v>
+      </c>
+      <c r="O13" s="16" t="s">
+        <v>36</v>
       </c>
       <c r="P13" s="17">
         <v>45951.0</v>
       </c>
       <c r="Q13" s="18">
-        <v>45965.0</v>
-      </c>
-      <c r="R13" s="12"/>
+        <v>45983.0</v>
+      </c>
+      <c r="R13" s="18">
+        <v>45968.0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="10" t="s">
         <v>37</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C14" s="12"/>
       <c r="D14" s="13">
@@ -1567,314 +1624,440 @@
       </c>
       <c r="E14" s="14">
         <f>Config!$B$2</f>
-        <v>1000</v>
+        <v>100000</v>
       </c>
       <c r="F14" s="14">
         <f t="shared" si="1"/>
-        <v>8000</v>
+        <v>800000</v>
       </c>
       <c r="G14" s="15">
         <v>1.0</v>
       </c>
       <c r="H14" s="14">
         <f t="shared" si="2"/>
-        <v>8000</v>
+        <v>800000</v>
       </c>
       <c r="I14" s="15">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J14" s="14">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K14" s="12"/>
+        <v>800000</v>
+      </c>
+      <c r="K14" s="15">
+        <v>350000.0</v>
+      </c>
       <c r="L14" s="14">
         <f t="shared" si="4"/>
-        <v>-8000</v>
+        <v>0</v>
       </c>
       <c r="M14" s="14">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="N14" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="O14" s="22" t="s">
-        <v>61</v>
+        <v>51</v>
+      </c>
+      <c r="O14" s="16" t="s">
+        <v>36</v>
       </c>
       <c r="P14" s="17">
         <v>45951.0</v>
       </c>
       <c r="Q14" s="18">
-        <v>45965.0</v>
-      </c>
-      <c r="R14" s="12"/>
+        <v>45984.0</v>
+      </c>
+      <c r="R14" s="17">
+        <v>45971.0</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="14">
-        <f>Config!$B$2</f>
-        <v>1000</v>
-      </c>
-      <c r="F15" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G15" s="12"/>
-      <c r="H15" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I15" s="12"/>
-      <c r="J15" s="14">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K15" s="12"/>
-      <c r="L15" s="14">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M15" s="14">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="12"/>
-      <c r="Q15" s="12"/>
-      <c r="R15" s="12"/>
+      <c r="A15" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="13">
+        <v>10.0</v>
+      </c>
+      <c r="E15" s="11">
+        <v>100000.0</v>
+      </c>
+      <c r="F15" s="11">
+        <v>1000000.0</v>
+      </c>
+      <c r="G15" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="H15" s="11">
+        <v>1000000.0</v>
+      </c>
+      <c r="I15" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="J15" s="11">
+        <v>1000000.0</v>
+      </c>
+      <c r="K15" s="11">
+        <v>950000.0</v>
+      </c>
+      <c r="L15" s="11">
+        <v>0.0</v>
+      </c>
+      <c r="M15" s="11">
+        <v>50000.0</v>
+      </c>
+      <c r="N15" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="O15" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="P15" s="19">
+        <v>45980.0</v>
+      </c>
+      <c r="Q15" s="19">
+        <v>45991.0</v>
+      </c>
+      <c r="R15" s="19">
+        <v>45990.0</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="14">
-        <f>Config!$B$2</f>
-        <v>1000</v>
-      </c>
-      <c r="F16" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="12"/>
-      <c r="H16" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I16" s="12"/>
-      <c r="J16" s="14">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K16" s="12"/>
-      <c r="L16" s="14">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M16" s="14">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="12"/>
-      <c r="R16" s="12"/>
+      <c r="A16" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="13">
+        <v>8.0</v>
+      </c>
+      <c r="E16" s="11">
+        <v>100000.0</v>
+      </c>
+      <c r="F16" s="11">
+        <v>800000.0</v>
+      </c>
+      <c r="G16" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="H16" s="11">
+        <v>800000.0</v>
+      </c>
+      <c r="I16" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="J16" s="11">
+        <v>800000.0</v>
+      </c>
+      <c r="K16" s="11">
+        <v>820000.0</v>
+      </c>
+      <c r="L16" s="11">
+        <v>0.0</v>
+      </c>
+      <c r="M16" s="11">
+        <v>-20000.0</v>
+      </c>
+      <c r="N16" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="O16" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="P16" s="19">
+        <v>45980.0</v>
+      </c>
+      <c r="Q16" s="19">
+        <v>45991.0</v>
+      </c>
+      <c r="R16" s="19">
+        <v>45991.0</v>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="14">
-        <f>Config!$B$2</f>
-        <v>1000</v>
-      </c>
-      <c r="F17" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G17" s="12"/>
-      <c r="H17" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I17" s="12"/>
-      <c r="J17" s="14">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K17" s="12"/>
-      <c r="L17" s="14">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M17" s="14">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="N17" s="12"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="12"/>
-      <c r="Q17" s="12"/>
-      <c r="R17" s="12"/>
+      <c r="A17" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="13">
+        <v>5.0</v>
+      </c>
+      <c r="E17" s="11">
+        <v>100000.0</v>
+      </c>
+      <c r="F17" s="11">
+        <v>500000.0</v>
+      </c>
+      <c r="G17" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="H17" s="11">
+        <v>500000.0</v>
+      </c>
+      <c r="I17" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="J17" s="11">
+        <v>500000.0</v>
+      </c>
+      <c r="K17" s="11">
+        <v>470000.0</v>
+      </c>
+      <c r="L17" s="11">
+        <v>0.0</v>
+      </c>
+      <c r="M17" s="11">
+        <v>30000.0</v>
+      </c>
+      <c r="N17" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="O17" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="P17" s="19">
+        <v>45980.0</v>
+      </c>
+      <c r="Q17" s="19">
+        <v>45991.0</v>
+      </c>
+      <c r="R17" s="19">
+        <v>45989.0</v>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="14">
-        <f>Config!$B$2</f>
-        <v>1000</v>
-      </c>
-      <c r="F18" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G18" s="12"/>
-      <c r="H18" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I18" s="12"/>
-      <c r="J18" s="14">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K18" s="12"/>
-      <c r="L18" s="14">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M18" s="14">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="N18" s="12"/>
-      <c r="O18" s="12"/>
-      <c r="P18" s="12"/>
-      <c r="Q18" s="12"/>
-      <c r="R18" s="12"/>
+      <c r="A18" s="20">
+        <v>37288.0</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="13">
+        <v>5.0</v>
+      </c>
+      <c r="E18" s="11">
+        <v>100000.0</v>
+      </c>
+      <c r="F18" s="11">
+        <v>500000.0</v>
+      </c>
+      <c r="G18" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="H18" s="11">
+        <v>500000.0</v>
+      </c>
+      <c r="I18" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="J18" s="11">
+        <v>500000.0</v>
+      </c>
+      <c r="K18" s="11">
+        <v>550000.0</v>
+      </c>
+      <c r="L18" s="11">
+        <v>0.0</v>
+      </c>
+      <c r="M18" s="11">
+        <v>-50000.0</v>
+      </c>
+      <c r="N18" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="O18" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="P18" s="19">
+        <v>45980.0</v>
+      </c>
+      <c r="Q18" s="19">
+        <v>45991.0</v>
+      </c>
+      <c r="R18" s="19">
+        <v>45988.0</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
+      <c r="A19" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>65</v>
+      </c>
       <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
+      <c r="D19" s="21">
+        <v>8.0</v>
+      </c>
       <c r="E19" s="14">
-        <f>Config!$B$2</f>
-        <v>1000</v>
+        <v>100000.0</v>
       </c>
       <c r="F19" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G19" s="12"/>
+        <v>800000.0</v>
+      </c>
+      <c r="G19" s="15">
+        <v>1.0</v>
+      </c>
       <c r="H19" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I19" s="12"/>
+        <v>800000.0</v>
+      </c>
+      <c r="I19" s="15">
+        <v>1.0</v>
+      </c>
       <c r="J19" s="14">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>800000.0</v>
       </c>
       <c r="K19" s="12"/>
-      <c r="L19" s="14">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M19" s="14">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="N19" s="12"/>
-      <c r="O19" s="12"/>
-      <c r="P19" s="12"/>
-      <c r="Q19" s="12"/>
-      <c r="R19" s="12"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="O19" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="P19" s="18">
+        <v>45992.0</v>
+      </c>
+      <c r="Q19" s="19">
+        <v>46006.0</v>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
+      <c r="A20" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>69</v>
+      </c>
       <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
+      <c r="D20" s="21">
+        <v>5.0</v>
+      </c>
       <c r="E20" s="14">
-        <f>Config!$B$2</f>
-        <v>1000</v>
+        <v>100000.0</v>
       </c>
       <c r="F20" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G20" s="12"/>
+        <v>500000.0</v>
+      </c>
+      <c r="G20" s="15">
+        <v>1.0</v>
+      </c>
       <c r="H20" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I20" s="12"/>
+        <v>500000.0</v>
+      </c>
+      <c r="I20" s="15">
+        <v>1.0</v>
+      </c>
       <c r="J20" s="14">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>500000.0</v>
       </c>
       <c r="K20" s="12"/>
-      <c r="L20" s="14">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M20" s="14">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="N20" s="12"/>
-      <c r="O20" s="12"/>
-      <c r="P20" s="12"/>
-      <c r="Q20" s="12"/>
-      <c r="R20" s="12"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="O20" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="P20" s="18">
+        <v>45992.0</v>
+      </c>
+      <c r="Q20" s="19">
+        <v>46006.0</v>
+      </c>
     </row>
     <row r="21">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
+      <c r="A21" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>71</v>
+      </c>
       <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
+      <c r="D21" s="21">
+        <v>8.0</v>
+      </c>
       <c r="E21" s="14">
-        <f>Config!$B$2</f>
-        <v>1000</v>
+        <v>100000.0</v>
       </c>
       <c r="F21" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G21" s="12"/>
+        <v>800000.0</v>
+      </c>
+      <c r="G21" s="15">
+        <v>1.0</v>
+      </c>
       <c r="H21" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I21" s="12"/>
+        <v>800000.0</v>
+      </c>
+      <c r="I21" s="15">
+        <v>1.0</v>
+      </c>
       <c r="J21" s="14">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>800000.0</v>
       </c>
       <c r="K21" s="12"/>
-      <c r="L21" s="14">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M21" s="14">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="N21" s="12"/>
-      <c r="O21" s="12"/>
-      <c r="P21" s="12"/>
-      <c r="Q21" s="12"/>
-      <c r="R21" s="12"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="O21" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="P21" s="18">
+        <v>45992.0</v>
+      </c>
+      <c r="Q21" s="19">
+        <v>46006.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" s="13">
+        <v>5.0</v>
+      </c>
+      <c r="E22" s="11">
+        <v>100000.0</v>
+      </c>
+      <c r="F22" s="11">
+        <v>500000.0</v>
+      </c>
+      <c r="G22" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="H22" s="11">
+        <v>500000.0</v>
+      </c>
+      <c r="I22" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="J22" s="11">
+        <v>500000.0</v>
+      </c>
+      <c r="N22" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="O22" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="P22" s="22">
+        <v>45992.0</v>
+      </c>
+      <c r="Q22" s="19">
+        <v>46006.0</v>
+      </c>
     </row>
     <row r="33">
       <c r="C33" s="23"/>
@@ -1994,7 +2177,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="5" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="B1" s="24" t="s">
         <v>12</v>
@@ -2002,37 +2185,38 @@
     </row>
     <row r="2">
       <c r="A2" s="25" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B2" s="7">
-        <f>SUM('WBS-EV'!H2:H1000)</f>
-        <v>54000</v>
+        <f>SUM('WBS-EV'!F2:F1000)</f>
+        <v>10800000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="25" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="B3" s="7">
-        <v>0.0</v>
+        <f>SUM('WBS-EV'!H2:H1000)</f>
+        <v>10800000</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="25" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="B4" s="7">
         <f>SUM('WBS-EV'!J2:J1000)</f>
-        <v>6000</v>
+        <v>10800000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="25" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="B5" s="7">
         <f>SUM('WBS-EV'!K2:K1000)</f>
-        <v>0</v>
+        <v>6300000</v>
       </c>
     </row>
     <row r="6">
@@ -2041,34 +2225,34 @@
     </row>
     <row r="7">
       <c r="A7" s="25" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="B7" s="7">
         <f>B4-B3</f>
-        <v>6000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="25" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="B8" s="7">
         <f>B4-B5</f>
-        <v>6000</v>
+        <v>4500000</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="B9" s="6" t="str">
+        <v>82</v>
+      </c>
+      <c r="B9" s="6">
         <f>IFERROR(B4/B3,"")</f>
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="25" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="B10" s="27" t="str">
         <f>IFERROR(B4/B5:"","")</f>
@@ -2077,7 +2261,7 @@
     </row>
     <row r="11">
       <c r="A11" s="25" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="B11" s="27" t="str">
         <f>IFERROR(B2/B10,"")</f>
@@ -2086,20 +2270,20 @@
     </row>
     <row r="12">
       <c r="A12" s="25" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="B12" s="27">
         <f>IFERROR(B11-B5,"")</f>
-        <v>0</v>
+        <v>-6300000</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="25" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="B13" s="27">
         <f>IFERROR(B2-B11,"")</f>
-        <v>54000</v>
+        <v>10800000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>